<commit_message>
Updated scan-code definitions for keyboard
</commit_message>
<xml_diff>
--- a/Resources/PS2ASCII.xlsx
+++ b/Resources/PS2ASCII.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="165">
   <si>
     <t>ESC</t>
   </si>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>SHIFT-ENTER</t>
+  </si>
+  <si>
+    <t>UP or 8</t>
+  </si>
+  <si>
+    <t>LEFT or 4</t>
+  </si>
+  <si>
+    <t>DOWN or 2</t>
+  </si>
+  <si>
+    <t>RIGHT or 6</t>
   </si>
 </sst>
 </file>
@@ -894,8 +906,8 @@
   <dimension ref="A1:J237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C219" sqref="C219"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J236" sqref="J2:J236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3729,7 +3741,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="1">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="C107" s="1">
         <v>69</v>
@@ -3752,7 +3764,7 @@
       </c>
       <c r="J107" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 49</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -3783,7 +3795,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="1">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>136</v>
@@ -3798,15 +3810,15 @@
       <c r="F109" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G109" s="1">
-        <v>4</v>
+      <c r="G109" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="H109" s="9" t="s">
         <v>144</v>
       </c>
       <c r="J109" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 52</v>
+        <v xml:space="preserve"> dc.b 6</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -3815,7 +3827,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>139</v>
@@ -3838,7 +3850,7 @@
       </c>
       <c r="J110" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 55</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -3913,7 +3925,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="1">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C114" s="1">
         <v>70</v>
@@ -3936,7 +3948,7 @@
       </c>
       <c r="J114" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 48</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -3977,7 +3989,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C116" s="1">
         <v>72</v>
@@ -3992,15 +4004,15 @@
       <c r="F116" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G116" s="1">
-        <v>2</v>
+      <c r="G116" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="H116" s="9" t="s">
         <v>144</v>
       </c>
       <c r="J116" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 50</v>
+        <v xml:space="preserve"> dc.b 5</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -4009,7 +4021,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="1">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C117" s="1">
         <v>73</v>
@@ -4032,7 +4044,7 @@
       </c>
       <c r="J117" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 53</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -4041,7 +4053,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="1">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C118" s="1">
         <v>74</v>
@@ -4056,15 +4068,15 @@
       <c r="F118" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G118" s="1">
-        <v>6</v>
+      <c r="G118" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="H118" s="9" t="s">
         <v>144</v>
       </c>
       <c r="J118" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 54</v>
+        <v xml:space="preserve"> dc.b 7</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -4073,7 +4085,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="1">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C119" s="1">
         <v>75</v>
@@ -4088,15 +4100,15 @@
       <c r="F119" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G119" s="1">
-        <v>8</v>
+      <c r="G119" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="H119" s="9" t="s">
         <v>144</v>
       </c>
       <c r="J119" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 56</v>
+        <v xml:space="preserve"> dc.b 4</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -4227,7 +4239,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="1">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>141</v>
@@ -4250,7 +4262,7 @@
       </c>
       <c r="J124" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 51</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -4320,7 +4332,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="1">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>140</v>
@@ -4343,7 +4355,7 @@
       </c>
       <c r="J127" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> dc.b 57</v>
+        <v xml:space="preserve"> dc.b 0</v>
       </c>
     </row>
     <row r="128" spans="1:10">

</xml_diff>